<commit_message>
fixes in context integration and new results for hyperparameter tuning and evaluation
</commit_message>
<xml_diff>
--- a/4_classification&evaluation/output/context_integration/evaluation_metrics.xlsx
+++ b/4_classification&evaluation/output/context_integration/evaluation_metrics.xlsx
@@ -562,76 +562,76 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.6672843742850605</v>
+        <v>0.6607870052619538</v>
       </c>
       <c r="C2" t="n">
-        <v>0.7088892234911315</v>
+        <v>0.7035922067296614</v>
       </c>
       <c r="D2" t="n">
-        <v>0.6672843742850605</v>
+        <v>0.6607870052619538</v>
       </c>
       <c r="E2" t="n">
-        <v>0.6662065631829821</v>
+        <v>0.6594390440119021</v>
       </c>
       <c r="F2" t="n">
-        <v>0.6995195607412492</v>
+        <v>0.6758636467627545</v>
       </c>
       <c r="G2" t="n">
-        <v>0.7354688905301465</v>
+        <v>0.7140070347185159</v>
       </c>
       <c r="H2" t="n">
-        <v>0.6995195607412492</v>
+        <v>0.6758636467627545</v>
       </c>
       <c r="I2" t="n">
-        <v>0.6972634051353677</v>
+        <v>0.6751043043023429</v>
       </c>
       <c r="J2" t="n">
-        <v>0.7080759551590025</v>
+        <v>0.6951727293525508</v>
       </c>
       <c r="K2" t="n">
-        <v>0.7534113441562489</v>
+        <v>0.7216533663203817</v>
       </c>
       <c r="L2" t="n">
-        <v>0.7080759551590025</v>
+        <v>0.6951727293525508</v>
       </c>
       <c r="M2" t="n">
-        <v>0.7099124329219381</v>
+        <v>0.6942983243939361</v>
       </c>
       <c r="N2" t="n">
-        <v>0.7123541523678791</v>
+        <v>0.7596202242049875</v>
       </c>
       <c r="O2" t="n">
-        <v>0.7421245055545139</v>
+        <v>0.7723836279450254</v>
       </c>
       <c r="P2" t="n">
-        <v>0.7123541523678791</v>
+        <v>0.7596202242049875</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.7108244891556594</v>
+        <v>0.758967210250951</v>
       </c>
       <c r="R2" t="n">
-        <v>0.7059025394646533</v>
+        <v>0.7617250057195151</v>
       </c>
       <c r="S2" t="n">
-        <v>0.738168318628652</v>
+        <v>0.7721246267043769</v>
       </c>
       <c r="T2" t="n">
-        <v>0.7059025394646533</v>
+        <v>0.7617250057195151</v>
       </c>
       <c r="U2" t="n">
-        <v>0.7045880123662341</v>
+        <v>0.7612488421848909</v>
       </c>
       <c r="V2" t="n">
-        <v>0.6887211164493251</v>
+        <v>0.7768474033401969</v>
       </c>
       <c r="W2" t="n">
-        <v>0.7247213883853493</v>
+        <v>0.7859811711427482</v>
       </c>
       <c r="X2" t="n">
-        <v>0.6887211164493251</v>
+        <v>0.7768474033401969</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.6879470654247306</v>
+        <v>0.7771016277200313</v>
       </c>
     </row>
     <row r="3">
@@ -641,76 +641,76 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.8069549302219172</v>
+        <v>0.8068862960420956</v>
       </c>
       <c r="C3" t="n">
-        <v>0.8189114424730277</v>
+        <v>0.8165817752422347</v>
       </c>
       <c r="D3" t="n">
-        <v>0.8069549302219172</v>
+        <v>0.8068862960420956</v>
       </c>
       <c r="E3" t="n">
-        <v>0.8074579526910645</v>
+        <v>0.8068985724823365</v>
       </c>
       <c r="F3" t="n">
-        <v>0.8090597117364448</v>
+        <v>0.8111873713109128</v>
       </c>
       <c r="G3" t="n">
-        <v>0.8212033276228496</v>
+        <v>0.8197327317326465</v>
       </c>
       <c r="H3" t="n">
-        <v>0.8090597117364448</v>
+        <v>0.8111873713109128</v>
       </c>
       <c r="I3" t="n">
-        <v>0.811267427939892</v>
+        <v>0.8127405508901064</v>
       </c>
       <c r="J3" t="n">
-        <v>0.8218714253031344</v>
+        <v>0.8240677190574239</v>
       </c>
       <c r="K3" t="n">
-        <v>0.8304473646044631</v>
+        <v>0.8341145190108777</v>
       </c>
       <c r="L3" t="n">
-        <v>0.8218714253031344</v>
+        <v>0.8240677190574239</v>
       </c>
       <c r="M3" t="n">
-        <v>0.8225533330830093</v>
+        <v>0.8242075632465828</v>
       </c>
       <c r="N3" t="n">
-        <v>0.8027224891329215</v>
+        <v>0.8477236330359185</v>
       </c>
       <c r="O3" t="n">
-        <v>0.8146369222698822</v>
+        <v>0.8563353892598808</v>
       </c>
       <c r="P3" t="n">
-        <v>0.8027224891329215</v>
+        <v>0.8477236330359185</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.8043005940055508</v>
+        <v>0.8477534818572938</v>
       </c>
       <c r="R3" t="n">
-        <v>0.8048730267673301</v>
+        <v>0.8498512926103867</v>
       </c>
       <c r="S3" t="n">
-        <v>0.8162781220435098</v>
+        <v>0.8581624833208151</v>
       </c>
       <c r="T3" t="n">
-        <v>0.8048730267673301</v>
+        <v>0.8498512926103867</v>
       </c>
       <c r="U3" t="n">
-        <v>0.8064418177407024</v>
+        <v>0.8498447448756513</v>
       </c>
       <c r="V3" t="n">
-        <v>0.8219171814230153</v>
+        <v>0.8498055364905056</v>
       </c>
       <c r="W3" t="n">
-        <v>0.8316948144271896</v>
+        <v>0.8559220440159205</v>
       </c>
       <c r="X3" t="n">
-        <v>0.8219171814230153</v>
+        <v>0.8498055364905056</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.823661274305738</v>
+        <v>0.8494250209424117</v>
       </c>
     </row>
     <row r="4">
@@ -720,76 +720,76 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.8455044612216884</v>
+        <v>0.8433310455273393</v>
       </c>
       <c r="C4" t="n">
-        <v>0.8509076213699405</v>
+        <v>0.8487473843105618</v>
       </c>
       <c r="D4" t="n">
-        <v>0.8455044612216884</v>
+        <v>0.8433310455273393</v>
       </c>
       <c r="E4" t="n">
-        <v>0.8458983843706773</v>
+        <v>0.8434160106629898</v>
       </c>
       <c r="F4" t="n">
-        <v>0.8755891100434683</v>
+        <v>0.8712880347746511</v>
       </c>
       <c r="G4" t="n">
-        <v>0.8816151258139827</v>
+        <v>0.8775425274847303</v>
       </c>
       <c r="H4" t="n">
-        <v>0.8755891100434683</v>
+        <v>0.8712880347746511</v>
       </c>
       <c r="I4" t="n">
-        <v>0.8757721115084423</v>
+        <v>0.871549669972255</v>
       </c>
       <c r="J4" t="n">
-        <v>0.8670098375657744</v>
+        <v>0.8498055364905056</v>
       </c>
       <c r="K4" t="n">
-        <v>0.8733510671745327</v>
+        <v>0.8564366739764255</v>
       </c>
       <c r="L4" t="n">
-        <v>0.8670098375657744</v>
+        <v>0.8498055364905056</v>
       </c>
       <c r="M4" t="n">
-        <v>0.8672413023802837</v>
+        <v>0.8502511645780464</v>
       </c>
       <c r="N4" t="n">
-        <v>0.8262640128117136</v>
+        <v>0.8541523678792039</v>
       </c>
       <c r="O4" t="n">
-        <v>0.8329565385703098</v>
+        <v>0.8589862301481432</v>
       </c>
       <c r="P4" t="n">
-        <v>0.8262640128117136</v>
+        <v>0.8541523678792039</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.8271284706265192</v>
+        <v>0.853473523710947</v>
       </c>
       <c r="R4" t="n">
-        <v>0.8262640128117136</v>
+        <v>0.8584534431480211</v>
       </c>
       <c r="S4" t="n">
-        <v>0.8329565385703098</v>
+        <v>0.8632781427252849</v>
       </c>
       <c r="T4" t="n">
-        <v>0.8262640128117136</v>
+        <v>0.8584534431480211</v>
       </c>
       <c r="U4" t="n">
-        <v>0.8271284706265192</v>
+        <v>0.8578926526236801</v>
       </c>
       <c r="V4" t="n">
-        <v>0.8347517730496454</v>
+        <v>0.8563029055136125</v>
       </c>
       <c r="W4" t="n">
-        <v>0.8442453922108859</v>
+        <v>0.8610149354238773</v>
       </c>
       <c r="X4" t="n">
-        <v>0.8347517730496454</v>
+        <v>0.8563029055136125</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.8357877769497429</v>
+        <v>0.8556654499841484</v>
       </c>
     </row>
     <row r="5">
@@ -799,28 +799,28 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.8390757263784032</v>
+        <v>0.8348204072294669</v>
       </c>
       <c r="C5" t="n">
-        <v>0.8497444560096697</v>
+        <v>0.8424913763141845</v>
       </c>
       <c r="D5" t="n">
-        <v>0.8390757263784032</v>
+        <v>0.8348204072294669</v>
       </c>
       <c r="E5" t="n">
-        <v>0.8374586063298777</v>
+        <v>0.8328226448728516</v>
       </c>
       <c r="F5" t="n">
-        <v>0.8476778769160376</v>
+        <v>0.8498055364905056</v>
       </c>
       <c r="G5" t="n">
-        <v>0.8584511983759375</v>
+        <v>0.8569006817846342</v>
       </c>
       <c r="H5" t="n">
-        <v>0.8476778769160376</v>
+        <v>0.8498055364905056</v>
       </c>
       <c r="I5" t="n">
-        <v>0.8465253800090917</v>
+        <v>0.8486362112405953</v>
       </c>
       <c r="J5" t="n">
         <v>0</v>
@@ -835,28 +835,28 @@
         <v>0</v>
       </c>
       <c r="N5" t="n">
-        <v>0.789773507206589</v>
+        <v>0.8347746511095859</v>
       </c>
       <c r="O5" t="n">
-        <v>0.8123513188442276</v>
+        <v>0.8453118490272775</v>
       </c>
       <c r="P5" t="n">
-        <v>0.789773507206589</v>
+        <v>0.8347746511095859</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.7876267153240436</v>
+        <v>0.8329856798001873</v>
       </c>
       <c r="R5" t="n">
-        <v>0.8090825897963854</v>
+        <v>0.8412262640128118</v>
       </c>
       <c r="S5" t="n">
-        <v>0.8219375292961628</v>
+        <v>0.8519692035217915</v>
       </c>
       <c r="T5" t="n">
-        <v>0.8090825897963854</v>
+        <v>0.8412262640128118</v>
       </c>
       <c r="U5" t="n">
-        <v>0.8083582184089859</v>
+        <v>0.8394283439992805</v>
       </c>
       <c r="V5" t="n">
         <v>0</v>
@@ -878,76 +878,76 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.8455502173415695</v>
+        <v>0.8541066117593228</v>
       </c>
       <c r="C6" t="n">
-        <v>0.8508333337242776</v>
+        <v>0.859921301250685</v>
       </c>
       <c r="D6" t="n">
-        <v>0.8455502173415695</v>
+        <v>0.8541066117593228</v>
       </c>
       <c r="E6" t="n">
-        <v>0.8451164043494905</v>
+        <v>0.8540234574043056</v>
       </c>
       <c r="F6" t="n">
-        <v>0.8606039807824297</v>
+        <v>0.8755891100434683</v>
       </c>
       <c r="G6" t="n">
-        <v>0.8661334229099644</v>
+        <v>0.8809666747163373</v>
       </c>
       <c r="H6" t="n">
-        <v>0.8606039807824297</v>
+        <v>0.8755891100434683</v>
       </c>
       <c r="I6" t="n">
-        <v>0.8606865914200459</v>
+        <v>0.8752460492178475</v>
       </c>
       <c r="J6" t="n">
-        <v>0.8434225577671013</v>
+        <v>0.8219171814230153</v>
       </c>
       <c r="K6" t="n">
-        <v>0.8564798576517616</v>
+        <v>0.8347579140389392</v>
       </c>
       <c r="L6" t="n">
-        <v>0.8434225577671013</v>
+        <v>0.8219171814230153</v>
       </c>
       <c r="M6" t="n">
-        <v>0.8451784425589406</v>
+        <v>0.8227163881853119</v>
       </c>
       <c r="N6" t="n">
-        <v>0.8133607870052619</v>
+        <v>0.8540837336993823</v>
       </c>
       <c r="O6" t="n">
-        <v>0.8201100888092512</v>
+        <v>0.8592373894203723</v>
       </c>
       <c r="P6" t="n">
-        <v>0.8133607870052619</v>
+        <v>0.8540837336993823</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.8144454003211992</v>
+        <v>0.85340309945919</v>
       </c>
       <c r="R6" t="n">
-        <v>0.8198352779684284</v>
+        <v>0.8519103180050331</v>
       </c>
       <c r="S6" t="n">
-        <v>0.8279514795455827</v>
+        <v>0.8594872292154676</v>
       </c>
       <c r="T6" t="n">
-        <v>0.8198352779684284</v>
+        <v>0.8519103180050331</v>
       </c>
       <c r="U6" t="n">
-        <v>0.8208256122704121</v>
+        <v>0.8510956953545248</v>
       </c>
       <c r="V6" t="n">
-        <v>0.8069778082818578</v>
+        <v>0.8519103180050331</v>
       </c>
       <c r="W6" t="n">
-        <v>0.8195316216567136</v>
+        <v>0.8563462984869019</v>
       </c>
       <c r="X6" t="n">
-        <v>0.8069778082818578</v>
+        <v>0.8519103180050331</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.8091227472925946</v>
+        <v>0.851092372017099</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final evaluation of requirements classification with context integration
</commit_message>
<xml_diff>
--- a/4_classification&evaluation/output/context_integration/evaluation_metrics.xlsx
+++ b/4_classification&evaluation/output/context_integration/evaluation_metrics.xlsx
@@ -586,16 +586,16 @@
         <v>0.6751043043023429</v>
       </c>
       <c r="J2" t="n">
-        <v>0.6951727293525508</v>
+        <v>0.6973690231068405</v>
       </c>
       <c r="K2" t="n">
-        <v>0.7216533663203817</v>
+        <v>0.7208591480536559</v>
       </c>
       <c r="L2" t="n">
-        <v>0.6951727293525508</v>
+        <v>0.6973690231068405</v>
       </c>
       <c r="M2" t="n">
-        <v>0.6942983243939361</v>
+        <v>0.6953594983715047</v>
       </c>
       <c r="N2" t="n">
         <v>0.7596202242049875</v>
@@ -610,28 +610,28 @@
         <v>0.758967210250951</v>
       </c>
       <c r="R2" t="n">
-        <v>0.7617250057195151</v>
+        <v>0.7660032029283916</v>
       </c>
       <c r="S2" t="n">
-        <v>0.7721246267043769</v>
+        <v>0.7760820378100716</v>
       </c>
       <c r="T2" t="n">
-        <v>0.7617250057195151</v>
+        <v>0.7660032029283916</v>
       </c>
       <c r="U2" t="n">
-        <v>0.7612488421848909</v>
+        <v>0.7654431671124573</v>
       </c>
       <c r="V2" t="n">
         <v>0.7768474033401969</v>
       </c>
       <c r="W2" t="n">
-        <v>0.7859811711427482</v>
+        <v>0.7877672318690958</v>
       </c>
       <c r="X2" t="n">
         <v>0.7768474033401969</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.7771016277200313</v>
+        <v>0.7772809472569253</v>
       </c>
     </row>
     <row r="3">
@@ -653,28 +653,28 @@
         <v>0.8068985724823365</v>
       </c>
       <c r="F3" t="n">
-        <v>0.8111873713109128</v>
+        <v>0.8133379089453214</v>
       </c>
       <c r="G3" t="n">
-        <v>0.8197327317326465</v>
+        <v>0.8218721920011042</v>
       </c>
       <c r="H3" t="n">
-        <v>0.8111873713109128</v>
+        <v>0.8133379089453214</v>
       </c>
       <c r="I3" t="n">
-        <v>0.8127405508901064</v>
+        <v>0.8147808147714887</v>
       </c>
       <c r="J3" t="n">
         <v>0.8240677190574239</v>
       </c>
       <c r="K3" t="n">
-        <v>0.8341145190108777</v>
+        <v>0.8331590494638522</v>
       </c>
       <c r="L3" t="n">
         <v>0.8240677190574239</v>
       </c>
       <c r="M3" t="n">
-        <v>0.8242075632465828</v>
+        <v>0.8247243502739942</v>
       </c>
       <c r="N3" t="n">
         <v>0.8477236330359185</v>
@@ -689,28 +689,28 @@
         <v>0.8477534818572938</v>
       </c>
       <c r="R3" t="n">
-        <v>0.8498512926103867</v>
+        <v>0.8519789521848548</v>
       </c>
       <c r="S3" t="n">
-        <v>0.8581624833208151</v>
+        <v>0.8598142707282346</v>
       </c>
       <c r="T3" t="n">
-        <v>0.8498512926103867</v>
+        <v>0.8519789521848548</v>
       </c>
       <c r="U3" t="n">
-        <v>0.8498447448756513</v>
+        <v>0.852081097935892</v>
       </c>
       <c r="V3" t="n">
-        <v>0.8498055364905056</v>
+        <v>0.8498284145504462</v>
       </c>
       <c r="W3" t="n">
-        <v>0.8559220440159205</v>
+        <v>0.8581762562608208</v>
       </c>
       <c r="X3" t="n">
-        <v>0.8498055364905056</v>
+        <v>0.8498284145504462</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.8494250209424117</v>
+        <v>0.8496333227015507</v>
       </c>
     </row>
     <row r="4">
@@ -732,28 +732,28 @@
         <v>0.8434160106629898</v>
       </c>
       <c r="F4" t="n">
-        <v>0.8712880347746511</v>
+        <v>0.8734385724090596</v>
       </c>
       <c r="G4" t="n">
-        <v>0.8775425274847303</v>
+        <v>0.8801279785676346</v>
       </c>
       <c r="H4" t="n">
-        <v>0.8712880347746511</v>
+        <v>0.8734385724090596</v>
       </c>
       <c r="I4" t="n">
-        <v>0.871549669972255</v>
+        <v>0.8738176868073346</v>
       </c>
       <c r="J4" t="n">
-        <v>0.8498055364905056</v>
+        <v>0.8433996797071609</v>
       </c>
       <c r="K4" t="n">
-        <v>0.8564366739764255</v>
+        <v>0.8505098024431348</v>
       </c>
       <c r="L4" t="n">
-        <v>0.8498055364905056</v>
+        <v>0.8433996797071609</v>
       </c>
       <c r="M4" t="n">
-        <v>0.8502511645780464</v>
+        <v>0.8440484512013443</v>
       </c>
       <c r="N4" t="n">
         <v>0.8541523678792039</v>
@@ -768,28 +768,28 @@
         <v>0.853473523710947</v>
       </c>
       <c r="R4" t="n">
-        <v>0.8584534431480211</v>
+        <v>0.8606039807824297</v>
       </c>
       <c r="S4" t="n">
-        <v>0.8632781427252849</v>
+        <v>0.8652903416814567</v>
       </c>
       <c r="T4" t="n">
-        <v>0.8584534431480211</v>
+        <v>0.8606039807824297</v>
       </c>
       <c r="U4" t="n">
-        <v>0.8578926526236801</v>
+        <v>0.8600211334618383</v>
       </c>
       <c r="V4" t="n">
-        <v>0.8563029055136125</v>
+        <v>0.8605811027224892</v>
       </c>
       <c r="W4" t="n">
-        <v>0.8610149354238773</v>
+        <v>0.8660553055821871</v>
       </c>
       <c r="X4" t="n">
-        <v>0.8563029055136125</v>
+        <v>0.8605811027224892</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.8556654499841484</v>
+        <v>0.8599587702034434</v>
       </c>
     </row>
     <row r="5">
@@ -835,16 +835,16 @@
         <v>0</v>
       </c>
       <c r="N5" t="n">
-        <v>0.8347746511095859</v>
+        <v>0.8369251887439946</v>
       </c>
       <c r="O5" t="n">
-        <v>0.8453118490272775</v>
+        <v>0.8474318443561014</v>
       </c>
       <c r="P5" t="n">
-        <v>0.8347746511095859</v>
+        <v>0.8369251887439946</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.8329856798001873</v>
+        <v>0.8351730171881542</v>
       </c>
       <c r="R5" t="n">
         <v>0.8412262640128118</v>
@@ -881,73 +881,73 @@
         <v>0.8541066117593228</v>
       </c>
       <c r="C6" t="n">
-        <v>0.859921301250685</v>
+        <v>0.8595629681419273</v>
       </c>
       <c r="D6" t="n">
         <v>0.8541066117593228</v>
       </c>
       <c r="E6" t="n">
-        <v>0.8540234574043056</v>
+        <v>0.8539852933423724</v>
       </c>
       <c r="F6" t="n">
-        <v>0.8755891100434683</v>
+        <v>0.8713109128345916</v>
       </c>
       <c r="G6" t="n">
-        <v>0.8809666747163373</v>
+        <v>0.8755292665935478</v>
       </c>
       <c r="H6" t="n">
-        <v>0.8755891100434683</v>
+        <v>0.8713109128345916</v>
       </c>
       <c r="I6" t="n">
-        <v>0.8752460492178475</v>
+        <v>0.8709376453541209</v>
       </c>
       <c r="J6" t="n">
-        <v>0.8219171814230153</v>
+        <v>0.8304735758407688</v>
       </c>
       <c r="K6" t="n">
-        <v>0.8347579140389392</v>
+        <v>0.8403918233504697</v>
       </c>
       <c r="L6" t="n">
-        <v>0.8219171814230153</v>
+        <v>0.8304735758407688</v>
       </c>
       <c r="M6" t="n">
-        <v>0.8227163881853119</v>
+        <v>0.8307894683990016</v>
       </c>
       <c r="N6" t="n">
-        <v>0.8540837336993823</v>
+        <v>0.8519331960649736</v>
       </c>
       <c r="O6" t="n">
-        <v>0.8592373894203723</v>
+        <v>0.8577064876295909</v>
       </c>
       <c r="P6" t="n">
-        <v>0.8540837336993823</v>
+        <v>0.8519331960649736</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.85340309945919</v>
+        <v>0.851240140726601</v>
       </c>
       <c r="R6" t="n">
-        <v>0.8519103180050331</v>
+        <v>0.8691603752001831</v>
       </c>
       <c r="S6" t="n">
-        <v>0.8594872292154676</v>
+        <v>0.874993950629074</v>
       </c>
       <c r="T6" t="n">
-        <v>0.8519103180050331</v>
+        <v>0.8691603752001831</v>
       </c>
       <c r="U6" t="n">
-        <v>0.8510956953545248</v>
+        <v>0.8685697322098177</v>
       </c>
       <c r="V6" t="n">
-        <v>0.8519103180050331</v>
+        <v>0.8540379775795014</v>
       </c>
       <c r="W6" t="n">
-        <v>0.8563462984869019</v>
+        <v>0.8589613235760376</v>
       </c>
       <c r="X6" t="n">
-        <v>0.8519103180050331</v>
+        <v>0.8540379775795014</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.851092372017099</v>
+        <v>0.853904858120757</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix in context integration and updated evaluation results
</commit_message>
<xml_diff>
--- a/4_classification&evaluation/output/context_integration/evaluation_metrics.xlsx
+++ b/4_classification&evaluation/output/context_integration/evaluation_metrics.xlsx
@@ -565,73 +565,73 @@
         <v>0.6607870052619538</v>
       </c>
       <c r="C2" t="n">
-        <v>0.7035922067296614</v>
+        <v>0.7020509200022044</v>
       </c>
       <c r="D2" t="n">
         <v>0.6607870052619538</v>
       </c>
       <c r="E2" t="n">
-        <v>0.6594390440119021</v>
+        <v>0.6591064774027398</v>
       </c>
       <c r="F2" t="n">
         <v>0.6758636467627545</v>
       </c>
       <c r="G2" t="n">
-        <v>0.7140070347185159</v>
+        <v>0.7159537408372849</v>
       </c>
       <c r="H2" t="n">
         <v>0.6758636467627545</v>
       </c>
       <c r="I2" t="n">
-        <v>0.6751043043023429</v>
+        <v>0.6754103730229087</v>
       </c>
       <c r="J2" t="n">
-        <v>0.6973690231068405</v>
+        <v>0.6736902310684053</v>
       </c>
       <c r="K2" t="n">
-        <v>0.7208591480536559</v>
+        <v>0.7207704319285049</v>
       </c>
       <c r="L2" t="n">
-        <v>0.6973690231068405</v>
+        <v>0.6736902310684053</v>
       </c>
       <c r="M2" t="n">
-        <v>0.6953594983715047</v>
+        <v>0.6812638326675795</v>
       </c>
       <c r="N2" t="n">
-        <v>0.7596202242049875</v>
+        <v>0.7617707618393961</v>
       </c>
       <c r="O2" t="n">
-        <v>0.7723836279450254</v>
+        <v>0.7746930423729357</v>
       </c>
       <c r="P2" t="n">
-        <v>0.7596202242049875</v>
+        <v>0.7617707618393961</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.758967210250951</v>
+        <v>0.7611321514088113</v>
       </c>
       <c r="R2" t="n">
-        <v>0.7660032029283916</v>
+        <v>0.7725692061313202</v>
       </c>
       <c r="S2" t="n">
-        <v>0.7760820378100716</v>
+        <v>0.7778172554919252</v>
       </c>
       <c r="T2" t="n">
-        <v>0.7660032029283916</v>
+        <v>0.7725692061313202</v>
       </c>
       <c r="U2" t="n">
-        <v>0.7654431671124573</v>
+        <v>0.7712238612542054</v>
       </c>
       <c r="V2" t="n">
-        <v>0.7768474033401969</v>
+        <v>0.7682452528025625</v>
       </c>
       <c r="W2" t="n">
-        <v>0.7877672318690958</v>
+        <v>0.7826359218639817</v>
       </c>
       <c r="X2" t="n">
-        <v>0.7768474033401969</v>
+        <v>0.7682452528025625</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.7772809472569253</v>
+        <v>0.7674291100701333</v>
       </c>
     </row>
     <row r="3">
@@ -641,76 +641,76 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.8068862960420956</v>
+        <v>0.8112102493708534</v>
       </c>
       <c r="C3" t="n">
-        <v>0.8165817752422347</v>
+        <v>0.8207966514864495</v>
       </c>
       <c r="D3" t="n">
-        <v>0.8068862960420956</v>
+        <v>0.8112102493708534</v>
       </c>
       <c r="E3" t="n">
-        <v>0.8068985724823365</v>
+        <v>0.8111071707280153</v>
       </c>
       <c r="F3" t="n">
-        <v>0.8133379089453214</v>
+        <v>0.8112102493708534</v>
       </c>
       <c r="G3" t="n">
-        <v>0.8218721920011042</v>
+        <v>0.8242138907844732</v>
       </c>
       <c r="H3" t="n">
-        <v>0.8133379089453214</v>
+        <v>0.8112102493708534</v>
       </c>
       <c r="I3" t="n">
-        <v>0.8147808147714887</v>
+        <v>0.8125024364594374</v>
       </c>
       <c r="J3" t="n">
-        <v>0.8240677190574239</v>
+        <v>0.8197208876687258</v>
       </c>
       <c r="K3" t="n">
-        <v>0.8331590494638522</v>
+        <v>0.8284665768499497</v>
       </c>
       <c r="L3" t="n">
-        <v>0.8240677190574239</v>
+        <v>0.8197208876687258</v>
       </c>
       <c r="M3" t="n">
-        <v>0.8247243502739942</v>
+        <v>0.8199223638417941</v>
       </c>
       <c r="N3" t="n">
-        <v>0.8477236330359185</v>
+        <v>0.8455730954015099</v>
       </c>
       <c r="O3" t="n">
-        <v>0.8563353892598808</v>
+        <v>0.8545911030801108</v>
       </c>
       <c r="P3" t="n">
-        <v>0.8477236330359185</v>
+        <v>0.8455730954015099</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.8477534818572938</v>
+        <v>0.8456102159964825</v>
       </c>
       <c r="R3" t="n">
-        <v>0.8519789521848548</v>
+        <v>0.8541294898192634</v>
       </c>
       <c r="S3" t="n">
-        <v>0.8598142707282346</v>
+        <v>0.8619421711243861</v>
       </c>
       <c r="T3" t="n">
-        <v>0.8519789521848548</v>
+        <v>0.8541294898192634</v>
       </c>
       <c r="U3" t="n">
-        <v>0.852081097935892</v>
+        <v>0.8541764935796747</v>
       </c>
       <c r="V3" t="n">
-        <v>0.8498284145504462</v>
+        <v>0.8541066117593228</v>
       </c>
       <c r="W3" t="n">
-        <v>0.8581762562608208</v>
+        <v>0.8615440293584173</v>
       </c>
       <c r="X3" t="n">
-        <v>0.8498284145504462</v>
+        <v>0.8541066117593228</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.8496333227015507</v>
+        <v>0.8539940367270453</v>
       </c>
     </row>
     <row r="4">
@@ -720,76 +720,76 @@
         </is>
       </c>
       <c r="B4" t="n">
+        <v>0.8368794326241135</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.8428092006304425</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.8368794326241135</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.837042800867278</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.8669869595058339</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.8733827777519755</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.8669869595058339</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.8672795407235553</v>
+      </c>
+      <c r="J4" t="n">
         <v>0.8433310455273393</v>
       </c>
-      <c r="C4" t="n">
-        <v>0.8487473843105618</v>
-      </c>
-      <c r="D4" t="n">
+      <c r="K4" t="n">
+        <v>0.849635434910638</v>
+      </c>
+      <c r="L4" t="n">
         <v>0.8433310455273393</v>
       </c>
-      <c r="E4" t="n">
-        <v>0.8434160106629898</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.8734385724090596</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.8801279785676346</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.8734385724090596</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0.8738176868073346</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0.8433996797071609</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0.8505098024431348</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0.8433996797071609</v>
-      </c>
       <c r="M4" t="n">
-        <v>0.8440484512013443</v>
+        <v>0.8436890525666965</v>
       </c>
       <c r="N4" t="n">
-        <v>0.8541523678792039</v>
+        <v>0.8498741706703271</v>
       </c>
       <c r="O4" t="n">
-        <v>0.8589862301481432</v>
+        <v>0.8566625970168582</v>
       </c>
       <c r="P4" t="n">
-        <v>0.8541523678792039</v>
+        <v>0.8498741706703271</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.853473523710947</v>
+        <v>0.8494232240342564</v>
       </c>
       <c r="R4" t="n">
-        <v>0.8606039807824297</v>
+        <v>0.8563257835735529</v>
       </c>
       <c r="S4" t="n">
-        <v>0.8652903416814567</v>
+        <v>0.8625464660246662</v>
       </c>
       <c r="T4" t="n">
-        <v>0.8606039807824297</v>
+        <v>0.8563257835735529</v>
       </c>
       <c r="U4" t="n">
-        <v>0.8600211334618383</v>
+        <v>0.8560758551987654</v>
       </c>
       <c r="V4" t="n">
-        <v>0.8605811027224892</v>
+        <v>0.8563257835735529</v>
       </c>
       <c r="W4" t="n">
-        <v>0.8660553055821871</v>
+        <v>0.8625464660246662</v>
       </c>
       <c r="X4" t="n">
-        <v>0.8605811027224892</v>
+        <v>0.8563257835735529</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.8599587702034434</v>
+        <v>0.8560758551987654</v>
       </c>
     </row>
     <row r="5">
@@ -811,16 +811,16 @@
         <v>0.8328226448728516</v>
       </c>
       <c r="F5" t="n">
-        <v>0.8498055364905056</v>
+        <v>0.8476778769160376</v>
       </c>
       <c r="G5" t="n">
-        <v>0.8569006817846342</v>
+        <v>0.8568907361680995</v>
       </c>
       <c r="H5" t="n">
-        <v>0.8498055364905056</v>
+        <v>0.8476778769160376</v>
       </c>
       <c r="I5" t="n">
-        <v>0.8486362112405953</v>
+        <v>0.8461502014655187</v>
       </c>
       <c r="J5" t="n">
         <v>0</v>
@@ -878,76 +878,76 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.8541066117593228</v>
+        <v>0.8476549988560971</v>
       </c>
       <c r="C6" t="n">
-        <v>0.8595629681419273</v>
+        <v>0.8540070616832077</v>
       </c>
       <c r="D6" t="n">
-        <v>0.8541066117593228</v>
+        <v>0.8476549988560971</v>
       </c>
       <c r="E6" t="n">
-        <v>0.8539852933423724</v>
+        <v>0.8474796938251774</v>
       </c>
       <c r="F6" t="n">
-        <v>0.8713109128345916</v>
+        <v>0.8734614504690003</v>
       </c>
       <c r="G6" t="n">
-        <v>0.8755292665935478</v>
+        <v>0.8782816257816257</v>
       </c>
       <c r="H6" t="n">
-        <v>0.8713109128345916</v>
+        <v>0.8734614504690003</v>
       </c>
       <c r="I6" t="n">
-        <v>0.8709376453541209</v>
+        <v>0.8735016000842328</v>
       </c>
       <c r="J6" t="n">
-        <v>0.8304735758407688</v>
+        <v>0.8305193319606496</v>
       </c>
       <c r="K6" t="n">
-        <v>0.8403918233504697</v>
+        <v>0.8429270116841419</v>
       </c>
       <c r="L6" t="n">
-        <v>0.8304735758407688</v>
+        <v>0.8305193319606496</v>
       </c>
       <c r="M6" t="n">
-        <v>0.8307894683990016</v>
+        <v>0.8326587172502233</v>
       </c>
       <c r="N6" t="n">
-        <v>0.8519331960649736</v>
+        <v>0.858361930908259</v>
       </c>
       <c r="O6" t="n">
-        <v>0.8577064876295909</v>
+        <v>0.8631156795488881</v>
       </c>
       <c r="P6" t="n">
-        <v>0.8519331960649736</v>
+        <v>0.858361930908259</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.851240140726601</v>
+        <v>0.8576040212183778</v>
       </c>
       <c r="R6" t="n">
-        <v>0.8691603752001831</v>
+        <v>0.8648821779913064</v>
       </c>
       <c r="S6" t="n">
-        <v>0.874993950629074</v>
+        <v>0.8712407940098277</v>
       </c>
       <c r="T6" t="n">
-        <v>0.8691603752001831</v>
+        <v>0.8648821779913064</v>
       </c>
       <c r="U6" t="n">
-        <v>0.8685697322098177</v>
+        <v>0.8643766410690196</v>
       </c>
       <c r="V6" t="n">
-        <v>0.8540379775795014</v>
+        <v>0.8519103180050331</v>
       </c>
       <c r="W6" t="n">
-        <v>0.8589613235760376</v>
+        <v>0.8554689458440858</v>
       </c>
       <c r="X6" t="n">
-        <v>0.8540379775795014</v>
+        <v>0.8519103180050331</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.853904858120757</v>
+        <v>0.8509369948730532</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
optimal n_neighbors parameter for kNN without feature selection or pca
</commit_message>
<xml_diff>
--- a/4_classification&evaluation/output/context_integration/evaluation_metrics.xlsx
+++ b/4_classification&evaluation/output/context_integration/evaluation_metrics.xlsx
@@ -562,16 +562,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.6607870052619538</v>
+        <v>0.6650652024708303</v>
       </c>
       <c r="C2" t="n">
-        <v>0.7020509200022044</v>
+        <v>0.727838722474945</v>
       </c>
       <c r="D2" t="n">
-        <v>0.6607870052619538</v>
+        <v>0.6650652024708303</v>
       </c>
       <c r="E2" t="n">
-        <v>0.6591064774027398</v>
+        <v>0.6637261923393825</v>
       </c>
       <c r="F2" t="n">
         <v>0.6758636467627545</v>
@@ -598,16 +598,16 @@
         <v>0.6812638326675795</v>
       </c>
       <c r="N2" t="n">
-        <v>0.7617707618393961</v>
+        <v>0.7874857012125374</v>
       </c>
       <c r="O2" t="n">
-        <v>0.7746930423729357</v>
+        <v>0.800592546381022</v>
       </c>
       <c r="P2" t="n">
-        <v>0.7617707618393961</v>
+        <v>0.7874857012125374</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.7611321514088113</v>
+        <v>0.7853567617702084</v>
       </c>
       <c r="R2" t="n">
         <v>0.7725692061313202</v>
@@ -893,37 +893,37 @@
         <v>0.8734614504690003</v>
       </c>
       <c r="G6" t="n">
-        <v>0.8782816257816257</v>
+        <v>0.8789981776696546</v>
       </c>
       <c r="H6" t="n">
         <v>0.8734614504690003</v>
       </c>
       <c r="I6" t="n">
-        <v>0.8735016000842328</v>
+        <v>0.8734765654573513</v>
       </c>
       <c r="J6" t="n">
-        <v>0.8305193319606496</v>
+        <v>0.8283687943262411</v>
       </c>
       <c r="K6" t="n">
-        <v>0.8429270116841419</v>
+        <v>0.8429374553699459</v>
       </c>
       <c r="L6" t="n">
-        <v>0.8305193319606496</v>
+        <v>0.8283687943262411</v>
       </c>
       <c r="M6" t="n">
-        <v>0.8326587172502233</v>
+        <v>0.8306296978538832</v>
       </c>
       <c r="N6" t="n">
         <v>0.858361930908259</v>
       </c>
       <c r="O6" t="n">
-        <v>0.8631156795488881</v>
+        <v>0.8629328911997162</v>
       </c>
       <c r="P6" t="n">
         <v>0.858361930908259</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.8576040212183778</v>
+        <v>0.8577187713252601</v>
       </c>
       <c r="R6" t="n">
         <v>0.8648821779913064</v>
@@ -938,16 +938,16 @@
         <v>0.8643766410690196</v>
       </c>
       <c r="V6" t="n">
-        <v>0.8519103180050331</v>
+        <v>0.8518874399450928</v>
       </c>
       <c r="W6" t="n">
-        <v>0.8554689458440858</v>
+        <v>0.8559014625503328</v>
       </c>
       <c r="X6" t="n">
-        <v>0.8519103180050331</v>
+        <v>0.8518874399450928</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.8509369948730532</v>
+        <v>0.8512286782416443</v>
       </c>
     </row>
   </sheetData>

</xml_diff>